<commit_message>
Full Project With Screenshot
</commit_message>
<xml_diff>
--- a/src/main/java/HRMDataFile.xlsx
+++ b/src/main/java/HRMDataFile.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15150" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="2520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="LeaveData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M22"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Tutorial</t>
   </si>
@@ -45,18 +44,6 @@
   </si>
   <si>
     <t>I need Leave</t>
-  </si>
-  <si>
-    <t>Odis Adalwin</t>
-  </si>
-  <si>
-    <t>US - Vacation</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Going Home</t>
   </si>
 </sst>
 </file>
@@ -411,7 +398,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,35 +437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2020</v>
-      </c>
-      <c r="H2" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>